<commit_message>
Update new tests and new testing result.
</commit_message>
<xml_diff>
--- a/Reports/Bug reports.xlsx
+++ b/Reports/Bug reports.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Resola_qa\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Resola_qa\Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5597BA14-D88F-4E9C-A52F-215FDF7E59C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7D82B3A-F74B-4650-AC02-70150A06C37A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
   <si>
     <t>#</t>
   </si>
@@ -70,6 +70,33 @@
   </si>
   <si>
     <t>Should not allow to update with app name's length is greater than 48 and we can not create new app in this case.</t>
+  </si>
+  <si>
+    <t>Issue type</t>
+  </si>
+  <si>
+    <t>Create shorten link - Missing validation when URL is null</t>
+  </si>
+  <si>
+    <t>Bug</t>
+  </si>
+  <si>
+    <t>Enhancement</t>
+  </si>
+  <si>
+    <t>POST api/v1/shorten</t>
+  </si>
+  <si>
+    <t>Should not allow generating shortCode if URL is null</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Disable app - response status code is 204 </t>
+  </si>
+  <si>
+    <t>Status code should be 200 to indicate that disable progress is successful.  204 is commonly used in GET method to indicate that record/data is not available</t>
+  </si>
+  <si>
+    <t>DELETE api/v1/apps</t>
   </si>
 </sst>
 </file>
@@ -117,11 +144,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -130,6 +154,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -411,91 +441,135 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:B5"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
-    <col min="2" max="2" width="76.42578125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="26.7109375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="35" style="2" customWidth="1"/>
-    <col min="5" max="5" width="42.140625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="76.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="26.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="35" style="1" customWidth="1"/>
+    <col min="6" max="6" width="42.140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
+    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
+    <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
+    <row r="4" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="5">
         <v>3</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="F4" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E5" s="4"/>
+    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6" s="5">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>